<commit_message>
queries de tudo ou nada - categoria-menção
</commit_message>
<xml_diff>
--- a/dados/analises/2024/excel/02-ranking-uf-tdn.xlsx
+++ b/dados/analises/2024/excel/02-ranking-uf-tdn.xlsx
@@ -83,13 +83,13 @@
     <t>MA</t>
   </si>
   <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
     <t>TO</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>MT</t>
   </si>
   <si>
     <t>RO</t>
@@ -849,7 +849,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>40604.341</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>17009.957</v>
@@ -883,12 +883,12 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -914,7 +914,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>40604.341</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>8504.978499999999</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>40604.341</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>10834.492</v>
@@ -1301,12 +1301,12 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1332,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>50</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>0</v>

</xml_diff>